<commit_message>
applied some font formatting to the excel output using openpyxl
</commit_message>
<xml_diff>
--- a/excel_automation/templates/template_project_parameters_all_fields.xlsx
+++ b/excel_automation/templates/template_project_parameters_all_fields.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="82">
   <si>
     <t xml:space="preserve">Planilha de Orçamento SINTÉTICA</t>
   </si>
@@ -262,12 +262,6 @@
   </si>
   <si>
     <t xml:space="preserve">QUADRO RESUMO DE COTAÇÕES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">POLICIA FEDERAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">THIAGO CARDINELLI</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -4178,10 +4172,10 @@
   <dimension ref="A2:C15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.57"/>
@@ -4197,21 +4191,21 @@
     </row>
     <row r="3" customFormat="false" ht="16.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="37" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="B3" s="37"/>
       <c r="C3" s="37"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="38" t="s">
-        <v>74</v>
+        <v>13</v>
       </c>
       <c r="B4" s="38"/>
       <c r="C4" s="38"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="39" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
@@ -4221,32 +4215,32 @@
         <v>53</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="41" t="s">
         <v>78</v>
-      </c>
-      <c r="B7" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="C7" s="41" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" s="43" t="s">
         <v>81</v>
-      </c>
-      <c r="B8" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="C8" s="43" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>